<commit_message>
split up AddInEvents moved config menu creation into ConfigFiles.vb improved Mapper
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF6645-2334-45FC-9458-18ED1CE55CC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72190610-95C6-46E0-93C2-9EEDDC331BE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="510" windowWidth="19710" windowHeight="8805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="510" windowWidth="19710" windowHeight="8805" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,15 @@
     <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$1</definedName>
     <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$2</definedName>
+    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$7</definedName>
     <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
     <definedName name="DBMapper">Example2!$A$1</definedName>
     <definedName name="DBMapper_employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="DBMapperDataRange">TestTable[TestId],TestTable[TestNum]</definedName>
+    <definedName name="DBMapperDataRange">TestTable[[#Headers],[TestId]]</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$2</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$8</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -134,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="178">
   <si>
     <t>0877</t>
   </si>
@@ -637,9 +636,6 @@
     <t>emp_id</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
     <t>TestStr</t>
   </si>
   <si>
@@ -658,7 +654,19 @@
     <t>TestId</t>
   </si>
   <si>
-    <t>test</t>
+    <t>dsfsdfsdfsd</t>
+  </si>
+  <si>
+    <t>rewrwer</t>
+  </si>
+  <si>
+    <t>werwer</t>
+  </si>
+  <si>
+    <t>zrtzrtz</t>
+  </si>
+  <si>
+    <t>rtzrtzrtzrtz</t>
   </si>
 </sst>
 </file>
@@ -710,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -718,7 +726,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -754,8 +761,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A1:D2" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A1:D8" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
@@ -2359,13 +2366,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -2382,20 +2391,20 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="G1" t="str">
         <f>_xll.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, no recalculation done for unchanged query...</v>
+        <v>Env:MSSQL, Retrieved 6 records from: Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2403,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="6">
         <v>32874</v>
@@ -2424,16 +2433,16 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="6">
         <v>43586</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>147</v>
       </c>
       <c r="G3" s="6"/>
@@ -2448,6 +2457,62 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43682</v>
+      </c>
+      <c r="D4" s="6">
+        <v>456.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43685</v>
+      </c>
+      <c r="D5" s="6">
+        <v>478.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43717</v>
+      </c>
+      <c r="D6" s="6">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43685</v>
+      </c>
+      <c r="D7" s="6">
+        <v>457.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2458,30 +2523,32 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
         <v>168</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>169</v>
-      </c>
-      <c r="D1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2489,13 +2556,94 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C2" s="3">
         <v>32874</v>
       </c>
       <c r="D2">
-        <v>14545.12</v>
+        <v>123.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43586</v>
+      </c>
+      <c r="D3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43682</v>
+      </c>
+      <c r="D4">
+        <v>456.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D5">
+        <v>478.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43717</v>
+      </c>
+      <c r="D6">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D7">
+        <v>457.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
on error -> try/catch
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72190610-95C6-46E0-93C2-9EEDDC331BE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="510" windowWidth="19710" windowHeight="8805" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="510" windowWidth="19710" windowHeight="8805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$1</definedName>
     <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$7</definedName>
+    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$3</definedName>
     <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
     <definedName name="DBMapper">Example2!$A$1</definedName>
     <definedName name="DBMapper_employee">Example1!$A$1:$H$47</definedName>
@@ -30,7 +24,7 @@
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,12 +40,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,12 +73,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,12 +96,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,15 +119,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="\\oebfa.co.at\admindfs\Home\rkapl\Documents\Meine Datenquellen\OEBFADBTVI00 ORE TestTable.odc" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" odcFile="\\oebfa.co.at\admindfs\Home\rkapl\Documents\Meine Datenquellen\OEBFADBTVI00 ORE TestTable.odc" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=ORE;Data Source=LENOVO-PC;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=00232441EA71;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;ORE&quot;.&quot;dbo&quot;.&quot;TestTable&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="179">
   <si>
     <t>0877</t>
   </si>
@@ -667,12 +661,15 @@
   </si>
   <si>
     <t>rtzrtzrtzrtz</t>
+  </si>
+  <si>
+    <t>TestID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -718,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -726,6 +723,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -748,7 +746,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -761,13 +759,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A1:D8" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A1:D8" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestId" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1062,14 +1060,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2364,17 +2362,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -2391,7 +2389,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>167</v>
@@ -2403,8 +2401,8 @@
         <v>169</v>
       </c>
       <c r="G1" t="str">
-        <f>_xll.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, Retrieved 6 records from: Select * FROM ORE..TestTable</v>
+        <f>_xll.DBAddin.Functions.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:Production, Retrieved 2 records from: Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2462,56 +2460,32 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="6">
-        <v>43682</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="7">
+        <v>43777</v>
       </c>
       <c r="D4" s="6">
-        <v>456.45</v>
+        <v>456.25</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="6">
-        <v>43685</v>
-      </c>
-      <c r="D5" s="6">
-        <v>478.32</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="6">
-        <v>43717</v>
-      </c>
-      <c r="D6" s="6">
-        <v>654</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="6">
-        <v>43685</v>
-      </c>
-      <c r="D7" s="6">
-        <v>457.5</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2521,11 +2495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added context create menus added OnSave decision in DBMapper added ignoreColumns in DBMapper
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -16,7 +16,7 @@
     <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$1</definedName>
     <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$3</definedName>
+    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$8</definedName>
     <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
     <definedName name="DBMapper">Example2!$A$1</definedName>
     <definedName name="DBMapper_employee">Example1!$A$1:$H$47</definedName>
@@ -87,7 +87,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>saveRangeToDB(, "TestTable", "TestID", "ORE", True)</t>
+          <t>saveRangeToDB(, "TestTable", "TestID", "ORE", True, ,"ignoredColumn", True)</t>
         </r>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="182">
   <si>
     <t>0877</t>
   </si>
@@ -664,6 +664,15 @@
   </si>
   <si>
     <t>TestID</t>
+  </si>
+  <si>
+    <t>cvb</t>
+  </si>
+  <si>
+    <t>ghfgh</t>
+  </si>
+  <si>
+    <t>ignoredColumn</t>
   </si>
 </sst>
 </file>
@@ -715,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -723,7 +732,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1060,7 +1068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2364,10 +2372,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2400,9 +2408,12 @@
       <c r="D1" s="4" t="s">
         <v>169</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="G1" t="str">
-        <f>_xll.DBAddin.Functions.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Production, Retrieved 2 records from: Select * FROM ORE..TestTable</v>
+        <f>_xll.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:Production, Retrieved 7 records from: Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2417,6 +2428,9 @@
       </c>
       <c r="D2" s="6">
         <v>123.9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -2443,6 +2457,9 @@
       <c r="D3" s="6">
         <v>147</v>
       </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2462,30 +2479,69 @@
       <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>43777</v>
       </c>
       <c r="D4" s="6">
         <v>456.25</v>
       </c>
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43685</v>
+      </c>
+      <c r="D5" s="6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43717</v>
+      </c>
+      <c r="D6" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43685</v>
+      </c>
+      <c r="D7" s="6">
+        <v>457.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43717</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed ignoreColumn problem added DBMapperCreate Support for ListObjects
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AF1795-AE3C-4189-A3AC-3C2A13EAACA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="510" windowWidth="19710" windowHeight="8805" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -16,15 +22,15 @@
     <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$1</definedName>
     <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$8</definedName>
+    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$11</definedName>
     <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
     <definedName name="DBMapper">Example2!$A$1</definedName>
-    <definedName name="DBMapper_employee">Example1!$A$1:$H$47</definedName>
+    <definedName name="DBMapper_employee">Example1!$A$1</definedName>
     <definedName name="DBMapperDataRange">TestTable[[#Headers],[TestId]]</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$8</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$11</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +38,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,12 +48,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -73,12 +81,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -96,12 +104,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -119,15 +127,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="\\oebfa.co.at\admindfs\Home\rkapl\Documents\Meine Datenquellen\OEBFADBTVI00 ORE TestTable.odc" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="\\oebfa.co.at\admindfs\Home\rkapl\Documents\Meine Datenquellen\OEBFADBTVI00 ORE TestTable.odc" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=ORE;Data Source=LENOVO-PC;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=00232441EA71;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;ORE&quot;.&quot;dbo&quot;.&quot;TestTable&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="185">
   <si>
     <t>0877</t>
   </si>
@@ -663,9 +671,6 @@
     <t>rtzrtzrtzrtz</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
     <t>cvb</t>
   </si>
   <si>
@@ -673,12 +678,24 @@
   </si>
   <si>
     <t>ignoredColumn</t>
+  </si>
+  <si>
+    <t>sdfsdfsdf</t>
+  </si>
+  <si>
+    <t>ertertert</t>
+  </si>
+  <si>
+    <t>fgdfgdfg</t>
+  </si>
+  <si>
+    <t>kjh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -724,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -732,6 +749,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -754,7 +772,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -767,13 +785,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A1:D8" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1068,20 +1086,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2370,17 +2388,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -2397,7 +2415,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>167</v>
@@ -2409,11 +2427,11 @@
         <v>169</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G1" t="str">
         <f>_xll.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Production, Retrieved 7 records from: Select * FROM ORE..TestTable</v>
+        <v>Env:MSSQL, Retrieved 10 records from: Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2430,7 +2448,7 @@
         <v>123.9</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -2458,7 +2476,7 @@
         <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -2477,16 +2495,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="C4" s="6">
-        <v>43777</v>
+        <v>43682</v>
       </c>
       <c r="D4" s="6">
-        <v>456.25</v>
+        <v>456.45</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -2541,7 +2559,52 @@
       <c r="C8" s="6">
         <v>43717</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="7">
+        <v>43748</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="7">
+        <v>43717</v>
+      </c>
+      <c r="D10" s="6">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="7">
+        <v>43685</v>
+      </c>
+      <c r="D11" s="6">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2551,12 +2614,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2675,6 +2738,48 @@
       <c r="C8" s="3">
         <v>43717</v>
       </c>
+      <c r="D8">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43717</v>
+      </c>
+      <c r="D10">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
got rid of Eventviewe log fixed DBRowFetch return message disabled query cache/refetch explicit ConnectionString setting reflected now in return of DBfunctions
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AF1795-AE3C-4189-A3AC-3C2A13EAACA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DB774-DAD8-4567-B685-1A5C62C1C828}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -741,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -749,7 +749,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2392,8 +2391,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2570,7 +2569,7 @@
       <c r="B9" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>43748</v>
       </c>
       <c r="D9" s="6"/>
@@ -2585,7 +2584,7 @@
       <c r="B10" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>43717</v>
       </c>
       <c r="D10" s="6">
@@ -2599,7 +2598,7 @@
       <c r="B11" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>43685</v>
       </c>
       <c r="D11" s="6">
@@ -2618,7 +2617,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed DBConcatCells Problems (no ToRange before, to avoid Excel race conditions) only one hostApp reference now documentation enhancement removed unnecessary project packages (ExcelDna.CellAddress and ExcelDna.RibbonFluent) added repairLegacyFunctions in Workbook_Open
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DB774-DAD8-4567-B685-1A5C62C1C828}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -19,18 +13,19 @@
   </sheets>
   <definedNames>
     <definedName name="DBFsource39344485625" hidden="1">#REF!</definedName>
-    <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$1</definedName>
+    <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$2</definedName>
+    <definedName name="DBFsource436715641890509" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget43642653946169" hidden="1">Example2!$A$1:$D$11</definedName>
+    <definedName name="DBFtarget436715641890509" hidden="1">Example2!$A$2:$D$10</definedName>
     <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
-    <definedName name="DBMapper">Example2!$A$1</definedName>
+    <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapper_employee">Example1!$A$1</definedName>
-    <definedName name="DBMapperDataRange">TestTable[[#Headers],[TestId]]</definedName>
+    <definedName name="DBMapperDataRange">TestTable[[#Headers],[TestID]]</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$1:$D$11</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$10</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,12 +43,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -81,12 +76,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,12 +99,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roland Kapl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,15 +122,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="\\oebfa.co.at\admindfs\Home\rkapl\Documents\Meine Datenquellen\OEBFADBTVI00 ORE TestTable.odc" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=ORE;Data Source=LENOVO-PC;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=00232441EA71;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;ORE&quot;.&quot;dbo&quot;.&quot;TestTable&quot;" commandType="3"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBPVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=InfoDB&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="181">
   <si>
     <t>0877</t>
   </si>
@@ -653,12 +648,6 @@
     <t>testtesttest</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
     <t>rewrwer</t>
   </si>
   <si>
@@ -680,23 +669,17 @@
     <t>ignoredColumn</t>
   </si>
   <si>
-    <t>sdfsdfsdf</t>
-  </si>
-  <si>
-    <t>ertertert</t>
-  </si>
-  <si>
-    <t>fgdfgdfg</t>
-  </si>
-  <si>
-    <t>kjh</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>ertert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -707,12 +690,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -771,7 +748,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -784,13 +761,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A1:D11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1085,14 +1062,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2387,17 +2364,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -2413,197 +2390,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" t="str">
+        <f>_xll.DBListFetch("select * from ORE..Testtable","",A2,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:Production, Retrieved 8 records from: select * from ORE..Testtable</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" t="str">
-        <f>_xll.DBListFetch("Select * FROM ORE..TestTable","",A1,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, Retrieved 10 records from: Select * FROM ORE..TestTable</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="6">
-        <v>32874</v>
-      </c>
-      <c r="D2" s="6">
-        <v>123.9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="6">
-        <v>43586</v>
+        <v>32874</v>
       </c>
       <c r="D3" s="6">
-        <v>147</v>
+        <v>123.9</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
+        <v>176</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C4" s="6">
-        <v>43682</v>
+        <v>43586</v>
       </c>
       <c r="D4" s="6">
-        <v>456.45</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6">
-        <v>43685</v>
+        <v>43777</v>
       </c>
       <c r="D5" s="6">
-        <v>478.32</v>
+        <v>456.25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C6" s="6">
-        <v>43717</v>
+        <v>43685</v>
       </c>
       <c r="D6" s="6">
-        <v>654</v>
+        <v>478.32</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C7" s="6">
-        <v>43685</v>
+        <v>43717</v>
       </c>
       <c r="D7" s="6">
-        <v>457.5</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C8" s="6">
-        <v>43717</v>
+        <v>43685</v>
       </c>
       <c r="D8" s="6">
-        <v>654</v>
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C9" s="6">
-        <v>43748</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" t="s">
-        <v>184</v>
+        <v>43717</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="6">
-        <v>43717</v>
-      </c>
-      <c r="D10" s="6">
-        <v>487</v>
-      </c>
+        <v>43685</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="6">
-        <v>43685</v>
-      </c>
-      <c r="D11" s="6">
-        <v>45</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2613,171 +2573,149 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" t="str">
+        <f>_xll.DBSetQuery("Select * FROM ORE..TestTable","",A2)</f>
+        <v>Env:Production, no recalculation done for unchanged query...</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>167</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>168</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="3">
-        <v>32874</v>
-      </c>
-      <c r="D2">
-        <v>123.9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="3">
-        <v>43586</v>
+        <v>32874</v>
       </c>
       <c r="D3">
-        <v>147</v>
+        <v>123.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C4" s="3">
-        <v>43682</v>
+        <v>43586</v>
       </c>
       <c r="D4">
-        <v>456.45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
-        <v>43685</v>
+        <v>43777</v>
       </c>
       <c r="D5">
-        <v>478.32</v>
+        <v>456.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C6" s="3">
-        <v>43717</v>
+        <v>43685</v>
       </c>
       <c r="D6">
-        <v>654</v>
+        <v>478.32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C7" s="3">
-        <v>43685</v>
+        <v>43717</v>
       </c>
       <c r="D7">
-        <v>457.5</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C8" s="3">
-        <v>43717</v>
+        <v>43685</v>
       </c>
       <c r="D8">
-        <v>654</v>
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C9" s="3">
-        <v>43748</v>
+        <v>43717</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D10">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="3">
         <v>43685</v>
-      </c>
-      <c r="D11">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of on error conversions to try/catch fixed logging added Intellisense for DB functions
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -12,18 +12,13 @@
     <sheet name="Example3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="DBFsource39344485625" hidden="1">#REF!</definedName>
-    <definedName name="DBFsource43642653946169" hidden="1">Example2!$G$2</definedName>
-    <definedName name="DBFsource436715641890509" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFsourcebooks" hidden="1">#REF!</definedName>
-    <definedName name="DBFtarget39344485625" hidden="1">#REF!,#REF!,#REF!</definedName>
-    <definedName name="DBFtarget436715641890509" hidden="1">Example2!$A$2:$D$10</definedName>
-    <definedName name="DBFtargetbooks" hidden="1">#REF!</definedName>
+    <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$11</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapper_employee">Example1!$A$1</definedName>
     <definedName name="DBMapperDataRange">TestTable[[#Headers],[TestID]]</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$10</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -130,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="182">
   <si>
     <t>0877</t>
   </si>
@@ -673,6 +668,9 @@
   </si>
   <si>
     <t>ertert</t>
+  </si>
+  <si>
+    <t>ttt</t>
   </si>
 </sst>
 </file>
@@ -761,8 +759,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D10" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D12" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D12"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
@@ -2369,14 +2367,15 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" customWidth="1"/>
@@ -2392,7 +2391,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable","",A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Production, Retrieved 8 records from: select * from ORE..Testtable</v>
+        <v>Env:Production, Retrieved 9 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2419,7 +2418,7 @@
       <c r="B3" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="2">
         <v>32874</v>
       </c>
       <c r="D3" s="6">
@@ -2447,7 +2446,7 @@
       <c r="B4" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="2">
         <v>43586</v>
       </c>
       <c r="D4" s="6">
@@ -2475,7 +2474,7 @@
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="2">
         <v>43777</v>
       </c>
       <c r="D5" s="6">
@@ -2492,7 +2491,7 @@
       <c r="B6" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>43685</v>
       </c>
       <c r="D6" s="6">
@@ -2506,7 +2505,7 @@
       <c r="B7" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>43717</v>
       </c>
       <c r="D7" s="6">
@@ -2520,7 +2519,7 @@
       <c r="B8" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="2">
         <v>43685</v>
       </c>
       <c r="D8" s="6">
@@ -2534,7 +2533,7 @@
       <c r="B9" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="2">
         <v>43717</v>
       </c>
       <c r="D9" s="6">
@@ -2548,20 +2547,30 @@
       <c r="B10" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>43685</v>
       </c>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43654</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>181</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
@@ -2575,10 +2584,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2718,6 +2727,26 @@
         <v>43685</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected new additions for DBAction/Sequences
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A9F2CB-ACCD-4877-AB72-2D4CDC0661D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -21,15 +15,15 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$13</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
-    <definedName name="DBMapper_employee">Example1!$A$1</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
+    <definedName name="DBMapperemployee">Example1!$A$1</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,108 +41,28 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Roland Kapl</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">saveRangeToDB(, "pubs",  "employee", "emp_id", True)
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Roland Kapl</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>saveRangeToDB(, "ORE", "TestTable", "TestID", True, ,"ignoredColumn", True)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>roland kapl</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{F821A6AB-83F4-4AA4-AECB-F52A378D38C5}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>saveRangeToDB(,"ORE","TestTable","TestID",True,"","",False)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>roland kapl</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E838203F-77A8-4DBB-8DDE-A49506ED1EBD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>DBAction(3,"ORE",True)</t>
-        </r>
-      </text>
+    <comment ref="A2" authorId="0">
+      <text/>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBPVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=InfoDB&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="182">
   <si>
     <t>0877</t>
   </si>
@@ -687,20 +601,20 @@
     <t>ignoredColumn</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
-    <t>Test,DataRange</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>ertert</t>
+  </si>
+  <si>
+    <t>ttt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -710,18 +624,6 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -778,7 +680,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -791,13 +693,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D13" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1092,14 +994,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2389,22 +2291,19 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2423,7 +2322,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable","",A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, Retrieved 7 records from: select * from ORE..Testtable</v>
+        <v>Env:Production, Retrieved 11 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2504,13 +2403,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2">
-        <v>43682</v>
+        <v>43777</v>
       </c>
       <c r="D5" s="6">
-        <v>456.45</v>
+        <v>456.25</v>
       </c>
       <c r="E5" t="s">
         <v>177</v>
@@ -2569,29 +2468,47 @@
         <v>43717</v>
       </c>
       <c r="D9" s="6">
-        <v>654</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43685</v>
+      </c>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43654</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>181</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
@@ -2617,22 +2534,21 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2641,7 +2557,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable","",A2)</f>
-        <v>Env:MSSQL, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:Production, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2691,13 +2607,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
-        <v>43682</v>
+        <v>43777</v>
       </c>
       <c r="D5">
-        <v>456.45</v>
+        <v>456.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2753,8 +2669,45 @@
         <v>43717</v>
       </c>
       <c r="D9">
-        <v>654</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2766,10 +2719,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F17163E-18FE-4589-A2FE-ECC1A31495CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2786,12 +2739,9 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>181</v>
-      </c>
+      <c r="A3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring, added clipboard legacy function handling
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -1005,7 +1005,7 @@
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2299,7 +2299,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2542,8 +2544,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
refactoring, tests, UI improvements
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,13 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$13</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$5</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$13</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -40,29 +40,16 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>roland kapl</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBPVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=InfoDB&quot;" command="Select * FROM ORE..TestTable"/>
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="174">
   <si>
     <t>0877</t>
   </si>
@@ -580,34 +567,10 @@
     <t>testtesttest</t>
   </si>
   <si>
-    <t>rewrwer</t>
+    <t>TestID</t>
   </si>
   <si>
     <t>werwer</t>
-  </si>
-  <si>
-    <t>zrtzrtz</t>
-  </si>
-  <si>
-    <t>rtzrtzrtzrtz</t>
-  </si>
-  <si>
-    <t>cvb</t>
-  </si>
-  <si>
-    <t>ghfgh</t>
-  </si>
-  <si>
-    <t>ignoredColumn</t>
-  </si>
-  <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>ertert</t>
-  </si>
-  <si>
-    <t>ttt</t>
   </si>
 </sst>
 </file>
@@ -693,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D13" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D5" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
@@ -994,7 +957,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1005,7 +968,7 @@
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2299,7 +2262,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2323,13 +2286,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>_xll.DBListFetch("select * from ORE..Testtable","",A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Production, Retrieved 11 records from: select * from ORE..Testtable</v>
+        <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:Development, Retrieved 3 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>167</v>
@@ -2340,9 +2303,7 @@
       <c r="D2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -2356,9 +2317,6 @@
       </c>
       <c r="D3" s="6">
         <v>123.9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>176</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2385,9 +2343,6 @@
       <c r="D4" s="6">
         <v>147</v>
       </c>
-      <c r="E4" t="s">
-        <v>176</v>
-      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -2405,112 +2360,55 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43777</v>
-      </c>
-      <c r="D5" s="6">
-        <v>456.25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>177</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D6" s="6">
-        <v>478.32</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D7" s="6">
-        <v>654</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D8" s="6">
-        <v>457.5</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="2">
-        <v>43685</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="2">
-        <v>43654</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>181</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
+      <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
@@ -2540,9 +2438,9 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2558,13 +2456,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>_xll.DBSetQuery("Select * FROM ORE..TestTable","",A2)</f>
-        <v>Env:Production, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
+        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
         <v>167</v>
@@ -2609,113 +2507,14 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43777</v>
-      </c>
-      <c r="D5">
-        <v>456.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D6">
-        <v>478.32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D7">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D8">
-        <v>457.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="3">
-        <v>43685</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="3">
-        <v>43654</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2724,17 +2523,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>"delete from ORE..TestTable where testID&gt;"&amp;B1</f>
-        <v>delete from ORE..TestTable where testID&gt;7</v>
+        <f>"delete from ORE..TestTable where TestID&gt;"&amp;B1</f>
+        <v>delete from ORE..TestTable where TestID&gt;7</v>
       </c>
       <c r="B1">
         <v>7</v>

</xml_diff>

<commit_message>
CommandButton for DBModif added
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -15,13 +15,13 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$5</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$6</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$5</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
   <si>
     <t>0877</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>werwer</t>
+  </si>
+  <si>
+    <t>etertert</t>
   </si>
 </sst>
 </file>
@@ -642,6 +645,56 @@
 </styleSheet>
 </file>
 
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>714375</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="CommandButton1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
@@ -656,8 +709,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D5" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D6" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D6"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
@@ -2258,12 +2311,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2287,7 +2340,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, Retrieved 3 records from: select * from ORE..Testtable</v>
+        <v>Env:Development, Retrieved 4 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2366,8 +2419,12 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>174</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6"/>
     </row>
@@ -2432,15 +2489,45 @@
       <c r="D16" s="6"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2511,16 +2598,28 @@
       </c>
       <c r="C5" s="3"/>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Enhanced Commundbuttons exception handling added
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22620363-39B6-45F6-9D74-436AF64DF83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
@@ -29,7 +23,7 @@
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$11</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,15 +41,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="178">
   <si>
     <t>0877</t>
   </si>
@@ -576,31 +570,25 @@
     <t>werwer</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
-    <t>rewrwer</t>
-  </si>
-  <si>
-    <t>zrtzrtz</t>
-  </si>
-  <si>
-    <t>rtzrtzrtzrtz</t>
-  </si>
-  <si>
-    <t>dfgdfgdfg</t>
-  </si>
-  <si>
-    <t>jhgjhgjh</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>etertert</t>
+  </si>
+  <si>
+    <t>jkhjkhjk</t>
+  </si>
+  <si>
+    <t>ertert</t>
+  </si>
+  <si>
+    <t>dfgdfg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -670,6 +658,26 @@
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -694,14 +702,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -709,20 +714,211 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="DBActionTest" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>247650</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="DBMapperTest" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>304800</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>876300</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="DBMapperemployee" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>723900</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>762000</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="DBSeqnceTest" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>323850</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="DBAction" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -734,7 +930,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -747,13 +943,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D11" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D11"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1048,20 +1244,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2349,17 +2545,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2378,7 +2574,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, Retrieved 9 records from: select * from ORE..Testtable</v>
+        <v>Env:Development, Retrieved 7 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2451,42 +2647,32 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43682</v>
-      </c>
-      <c r="D5" s="6">
-        <v>456.45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D6" s="6">
-        <v>478.32</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D7" s="6">
-        <v>654</v>
-      </c>
+        <v>43590</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -2496,11 +2682,9 @@
         <v>176</v>
       </c>
       <c r="C8" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D8" s="6">
-        <v>457.5</v>
-      </c>
+        <v>43653</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -2509,37 +2693,19 @@
       <c r="B9" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D9" s="6">
-        <v>654</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D10" s="6">
-        <v>45</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="2">
-        <v>43653</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -2581,8 +2747,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="DBMapper">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="1030" r:id="rId4" name="DBAction">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>323850</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId4" name="DBAction"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId6" name="DBSeqnceTest">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>762000</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId6" name="DBSeqnceTest"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId8" name="DBMapperemployee">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>304800</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId8" name="DBMapperemployee"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId10" name="DBMapperTest">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId10" name="DBMapperTest"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId12" name="DBActionTest">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>333375</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId12" name="DBActionTest"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId14" name="DBMapper">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -2601,7 +2892,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
+        <control shapeId="1025" r:id="rId14" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2609,7 +2900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -2619,7 +2910,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2628,7 +2919,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:MSSQL, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2678,41 +2969,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43682</v>
-      </c>
-      <c r="D5">
-        <v>456.45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D6">
-        <v>478.32</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C7" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D7">
-        <v>654</v>
+        <v>43590</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2723,10 +3001,7 @@
         <v>176</v>
       </c>
       <c r="C8" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D8">
-        <v>457.5</v>
+        <v>43653</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2736,37 +3011,22 @@
       <c r="B9" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D9">
-        <v>654</v>
-      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D10">
-        <v>45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="3">
-        <v>43653</v>
-      </c>
+      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2779,7 +3039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed severe bug in ToRange improved check for multiple execOnSave
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557EE6A-F66D-417C-900C-CA9D1E2C9195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -15,15 +21,15 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$10</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$11</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$10</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,15 +47,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="178">
   <si>
     <t>0877</t>
   </si>
@@ -570,25 +576,25 @@
     <t>werwer</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>etertert</t>
-  </si>
-  <si>
-    <t>jkhjkhjk</t>
-  </si>
-  <si>
-    <t>ertert</t>
-  </si>
-  <si>
-    <t>dfgdfg</t>
+    <t>TestId</t>
+  </si>
+  <si>
+    <t>dsfsdfsdfsd</t>
+  </si>
+  <si>
+    <t>rewrwer</t>
+  </si>
+  <si>
+    <t>zrtzrtz</t>
+  </si>
+  <si>
+    <t>rtzrtzrtzrtz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -680,16 +686,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>714375</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -698,11 +704,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -710,6 +719,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -721,16 +744,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -739,11 +762,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -751,6 +777,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -762,16 +802,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>466725</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -780,11 +820,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -792,6 +835,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -803,16 +860,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>876300</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -821,11 +878,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -833,6 +893,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -844,16 +918,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>723900</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>762000</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>476250</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -862,11 +936,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -874,6 +951,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -885,7 +976,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -898,13 +989,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1199,14 +1290,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2500,17 +2591,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2529,7 +2620,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, Retrieved 9 records from: select * from ORE..Testtable</v>
+        <v>Env:MSSQL, Retrieved 8 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2602,32 +2693,42 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+        <v>174</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43682</v>
+      </c>
+      <c r="D5" s="6">
+        <v>456.45</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43685</v>
+      </c>
+      <c r="D6" s="6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C7" s="2">
-        <v>43590</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>43717</v>
+      </c>
+      <c r="D7" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -2637,9 +2738,11 @@
         <v>176</v>
       </c>
       <c r="C8" s="2">
-        <v>43653</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>43685</v>
+      </c>
+      <c r="D8" s="6">
+        <v>457.5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -2648,23 +2751,23 @@
       <c r="B9" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="2">
+        <v>43717</v>
+      </c>
+      <c r="D9" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>172</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
+      <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
@@ -2712,16 +2815,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>714375</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2737,16 +2840,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2762,16 +2865,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>466725</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2787,16 +2890,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>876300</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2812,16 +2915,16 @@
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>762000</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2836,17 +2939,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2855,7 +2958,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:MSSQL, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2905,28 +3008,41 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43682</v>
+      </c>
+      <c r="D5">
+        <v>456.45</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C7" s="3">
-        <v>43590</v>
+        <v>43717</v>
+      </c>
+      <c r="D7">
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2937,7 +3053,10 @@
         <v>176</v>
       </c>
       <c r="C8" s="3">
-        <v>43653</v>
+        <v>43685</v>
+      </c>
+      <c r="D8">
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2947,22 +3066,18 @@
       <c r="B9" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>43717</v>
+      </c>
+      <c r="D9">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2975,11 +3090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed ignoring of MaxDepth in ConfigFile reading fixed unhandled exception in DBMapper fixed incorrect handling of intersections of formula range & target range in DBListFetchAction
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557EE6A-F66D-417C-900C-CA9D1E2C9195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -21,15 +15,15 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$10</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$10</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,9 +41,9 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
@@ -576,25 +570,25 @@
     <t>werwer</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
-    <t>rewrwer</t>
-  </si>
-  <si>
-    <t>zrtzrtz</t>
-  </si>
-  <si>
-    <t>rtzrtzrtzrtz</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>etertert</t>
+  </si>
+  <si>
+    <t>jkhjkhjk</t>
+  </si>
+  <si>
+    <t>ertert</t>
+  </si>
+  <si>
+    <t>dfgdfg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -704,14 +698,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -719,20 +710,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -762,14 +739,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -777,20 +751,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -803,31 +763,28 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9524</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>466725</xdr:colOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="DBMapperTest" hidden="1">
+            <xdr:cNvPr id="1027" name="DBMapperDataRange" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -835,20 +792,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -878,14 +821,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -893,20 +833,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -936,14 +862,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -951,20 +874,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -976,7 +885,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -989,13 +898,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D10" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1290,14 +1199,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2591,17 +2500,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2620,7 +2529,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, Retrieved 8 records from: select * from ORE..Testtable</v>
+        <v>Env:Development, Retrieved 7 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2693,42 +2602,32 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43682</v>
-      </c>
-      <c r="D5" s="6">
-        <v>456.45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D6" s="6">
-        <v>478.32</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D7" s="6">
-        <v>654</v>
-      </c>
+        <v>43590</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -2738,11 +2637,9 @@
         <v>176</v>
       </c>
       <c r="C8" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D8" s="6">
-        <v>457.5</v>
-      </c>
+        <v>43653</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -2751,17 +2648,11 @@
       <c r="B9" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D9" s="6">
-        <v>654</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
+      <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
@@ -2811,8 +2702,108 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="DBMapper">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId8" name="DBMapperDataRange">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>381000</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId8" name="DBMapperDataRange"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId10" name="DBActionTest">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId12" name="DBMapper">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2831,107 +2822,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="DBActionTest">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId8" name="DBMapperTest">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>466725</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId8" name="DBMapperTest"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2939,9 +2830,9 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -2949,7 +2840,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2958,7 +2849,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:MSSQL, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3008,41 +2899,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43682</v>
-      </c>
-      <c r="D5">
-        <v>456.45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D6">
-        <v>478.32</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C7" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D7">
-        <v>654</v>
+        <v>43590</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3053,10 +2931,7 @@
         <v>176</v>
       </c>
       <c r="C8" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D8">
-        <v>457.5</v>
+        <v>43653</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3066,18 +2941,7 @@
       <c r="B9" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D9">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3"/>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3090,11 +2954,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added DBrefresh (of DBListfetch and DBSetQuery functions) for DBSequences added DBtarget/DBsource for DBSetQuery (required for above and for jump functionality)
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,9 @@
   <definedNames>
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
+    <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
     <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
     <definedName name="DBMapper">Example2!$A$2</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1</definedName>
@@ -763,7 +765,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>9524</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
@@ -2504,8 +2506,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2703,7 +2705,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2728,7 +2730,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2753,7 +2755,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1027" r:id="rId8" name="DBMapperDataRange">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2778,7 +2780,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1026" r:id="rId10" name="DBActionTest">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2803,7 +2805,7 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1025" r:id="rId12" name="DBMapper">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -2834,8 +2836,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed DBModification to only 3 Buttons (for the three types). internal refactoring...
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
     <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
     <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapper">Example2!$A$2</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2</definedName>
-    <definedName name="DBMapperemployee">Example1!$A$1</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
+    <definedName name="DBMapperemployee">Example1!$A$1:$H$47</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
+    <definedName name="werwer">Example3!$G$17</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
   <si>
     <t>0877</t>
   </si>
@@ -585,6 +586,9 @@
   </si>
   <si>
     <t>dfgdfg</t>
+  </si>
+  <si>
+    <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1205,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1214,7 +1218,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2506,8 +2510,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2531,7 +2535,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, Retrieved 7 records from: select * from ORE..Testtable</v>
+        <v>Env:Development, (last result:)Retrieved 7 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2704,52 +2708,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
+        <control shapeId="1025" r:id="rId4" name="DBMapper">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
+        <control shapeId="1026" r:id="rId6" name="DBActionTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
+        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2779,52 +2783,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId10" name="DBActionTest">
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId12" name="DBMapper">
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2834,10 +2838,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2848,13 +2852,13 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2882,7 +2886,7 @@
         <v>123.9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2896,7 +2900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2905,7 +2909,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2914,7 +2918,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2936,7 +2940,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2944,6 +2948,11 @@
         <v>177</v>
       </c>
       <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2961,7 +2970,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added confirmation possibility command button create is now a button some refactoring and bug fixes env is now only in doDBModif, class wide env obtained by getEnv
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD1256C-8087-441E-AD72-4BD5F9ABD91B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="780" yWindow="540" windowWidth="15870" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -16,17 +22,18 @@
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
-    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$12</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$12</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$12</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$12</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$47</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$12</definedName>
     <definedName name="werwer">Example3!$G$17</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,15 +51,37 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="180">
   <si>
     <t>0877</t>
   </si>
@@ -573,28 +602,31 @@
     <t>werwer</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>etertert</t>
-  </si>
-  <si>
-    <t>jkhjkhjk</t>
-  </si>
-  <si>
-    <t>ertert</t>
-  </si>
-  <si>
-    <t>dfgdfg</t>
-  </si>
-  <si>
     <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
+  </si>
+  <si>
+    <t>TestId</t>
+  </si>
+  <si>
+    <t>dsfsdfsdfsd</t>
+  </si>
+  <si>
+    <t>rewrwer</t>
+  </si>
+  <si>
+    <t>zrtzrtz</t>
+  </si>
+  <si>
+    <t>rtzrtzrtzrtz</t>
+  </si>
+  <si>
+    <t>fghfghfgh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -704,11 +736,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -716,6 +751,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -745,11 +794,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -757,6 +809,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -786,11 +852,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -798,6 +867,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -827,11 +910,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -839,6 +925,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -868,11 +968,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -880,6 +983,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -891,7 +1008,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -904,13 +1021,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D12" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1205,20 +1322,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2506,17 +2623,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2533,14 +2650,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="str">
-        <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, (last result:)Retrieved 7 records from: select * from ORE..Testtable</v>
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1">_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:MSSQL, (last result:)Retrieved 10 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>167</v>
@@ -2608,69 +2725,93 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43682</v>
+      </c>
+      <c r="D5" s="6">
+        <v>456.45</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
+        <v>176</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43685</v>
+      </c>
+      <c r="D6" s="6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C7" s="2">
-        <v>43590</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>43717</v>
+      </c>
+      <c r="D7" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="2">
-        <v>43653</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>43685</v>
+      </c>
+      <c r="D8" s="6">
+        <v>457.5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
+        <v>178</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43717</v>
+      </c>
+      <c r="D9" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>179</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
@@ -2836,31 +2977,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="str">
-        <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1">_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
         <v>167</v>
@@ -2905,28 +3046,41 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43682</v>
+      </c>
+      <c r="D5">
+        <v>456.45</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C7" s="3">
-        <v>43590</v>
+        <v>43717</v>
+      </c>
+      <c r="D7">
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2934,10 +3088,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="3">
-        <v>43653</v>
+        <v>43685</v>
+      </c>
+      <c r="D8">
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2945,14 +3102,38 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43717</v>
+      </c>
+      <c r="D9">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="3"/>
       <c r="G10" t="s">
-        <v>178</v>
-      </c>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2965,7 +3146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed position problem in EditDBModifDef fixed primkey case problem fixed update of empty fields
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD1256C-8087-441E-AD72-4BD5F9ABD91B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBF3295-CA1C-42BC-8968-5BE4D9BFF50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="540" windowWidth="15870" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,15 @@
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$12</definedName>
-    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$12</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$12</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2:$D$12</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$47</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$12</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
     <definedName name="werwer">Example3!$G$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
   <si>
     <t>0877</t>
   </si>
@@ -618,9 +618,6 @@
   </si>
   <si>
     <t>rtzrtzrtzrtz</t>
-  </si>
-  <si>
-    <t>fghfghfgh</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1018,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D12" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
@@ -2650,9 +2647,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1">_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, (last result:)Retrieved 10 records from: select * from ORE..Testtable</v>
+      <c r="A1" t="e" cm="1">
+        <f t="array" aca="1" ref="A1" ca="1">_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2791,27 +2788,19 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>179</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
+      <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
+      <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
@@ -2849,52 +2838,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="DBMapper">
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="DBActionTest">
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2924,52 +2913,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
+        <control shapeId="1026" r:id="rId10" name="DBActionTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
+        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
+        <control shapeId="1025" r:id="rId12" name="DBMapper">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2979,7 +2968,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -2994,9 +2983,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1">_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+      <c r="A1" t="e" cm="1">
+        <f t="array" aca="1" ref="A1" ca="1">_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3112,28 +3101,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="3"/>
       <c r="G10" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3174,4 +3144,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<root xmlns="DBModifDef">
+  <DBActionTest>
+    <env>3</env>
+    <database>ORE</database>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBActionTest>
+  <DBMapperemployee>
+    <env>3</env>
+    <database>pubs</database>
+    <tableName>employee</tableName>
+    <primKeysStr>emp_id</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns/>
+    <execOnSave>False</execOnSave>
+    <CUDFlags>False</CUDFlags>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapperemployee>
+  <DBMapperDataRange>
+    <env>3</env>
+    <database>ORE</database>
+    <tableName>TestTable</tableName>
+    <primKeysStr>TestID</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns/>
+    <execOnSave>False</execOnSave>
+    <CUDFlags>False</CUDFlags>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapperDataRange>
+  <DBSeqnceTest>
+    <execOnSave>True</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+    <seqStep>DBAction:DBActionTest</seqStep>
+    <seqStep>DBMapper:DBMapperDataRange</seqStep>
+  </DBSeqnceTest>
+  <DBSeqncetestRefresh>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+    <seqStep>DBMapper:DBMapperDataRange</seqStep>
+    <seqStep>DBRefrsh:DBFsource436717175553588:DBListFetch(in Example2!$A$1)</seqStep>
+  </DBSeqncetestRefresh>
+  <DBMapper>
+    <env/>
+    <database>ORE</database>
+    <tableName>TestTable</tableName>
+    <primKeysStr>TestID</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns>ignoredColumn</ignoreColumns>
+    <execOnSave>False</execOnSave>
+    <CUDFlags>False</CUDFlags>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapper>
+</root>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60067F7C-9141-4335-856F-A5078F7B86EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="DBModifDef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed problem with resizing DBMapper in non active workbook. reduced refresh by only removing cacheQueries and StatusCollections from active workbook.
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBF3295-CA1C-42BC-8968-5BE4D9BFF50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -24,16 +18,15 @@
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
     <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
     <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$E$9</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapperemployee">Example1!$A$1:$H$47</definedName>
+    <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
     <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="werwer">Example3!$G$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,37 +44,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="185">
   <si>
     <t>0877</t>
   </si>
@@ -605,25 +576,43 @@
     <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
-    <t>rewrwer</t>
-  </si>
-  <si>
-    <t>zrtzrtz</t>
-  </si>
-  <si>
-    <t>rtzrtzrtzrtz</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>etertert</t>
+  </si>
+  <si>
+    <t>jkhjkhjk</t>
+  </si>
+  <si>
+    <t>ertert</t>
+  </si>
+  <si>
+    <t>ignoredColumn</t>
+  </si>
+  <si>
+    <t>ert</t>
+  </si>
+  <si>
+    <t>erte</t>
+  </si>
+  <si>
+    <t>rtzrfh</t>
+  </si>
+  <si>
+    <t>DZT39436F</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>AAAA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -733,14 +722,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -748,20 +734,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -791,14 +763,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -806,20 +775,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -849,14 +804,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -864,20 +816,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -907,14 +845,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -922,20 +857,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -965,14 +886,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -980,20 +898,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1005,7 +909,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -1018,13 +922,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1319,20 +1223,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2604,6 +2508,27 @@
       <c r="S47" s="2"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48" t="s">
+        <v>181</v>
+      </c>
+      <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>170</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="2">
+        <v>40001</v>
+      </c>
       <c r="S48" s="3"/>
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.2">
@@ -2620,17 +2545,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2647,9 +2572,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="e" cm="1">
-        <f t="array" aca="1" ref="A1" ca="1">_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>#VALUE!</v>
+      <c r="A1" t="str">
+        <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
+        <v>Env:Development, (last result:)Retrieved 7 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2665,7 +2590,9 @@
       <c r="D2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -2679,6 +2606,9 @@
       </c>
       <c r="D3" s="6">
         <v>123.9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2705,6 +2635,9 @@
       <c r="D4" s="6">
         <v>147</v>
       </c>
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -2722,13 +2655,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43682</v>
-      </c>
-      <c r="D5" s="6">
-        <v>456.45</v>
+        <v>172</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
+      <c r="E5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -2736,13 +2668,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D6" s="6">
-        <v>478.32</v>
+        <v>175</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+      <c r="E6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -2750,14 +2681,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C7" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D7" s="6">
-        <v>654</v>
-      </c>
+        <v>43590</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -2767,25 +2696,19 @@
         <v>177</v>
       </c>
       <c r="C8" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D8" s="6">
-        <v>457.5</v>
-      </c>
+        <v>43653</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D9" s="6">
-        <v>654</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
@@ -2966,26 +2889,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="e" cm="1">
-        <f t="array" aca="1" ref="A1" ca="1">_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>#VALUE!</v>
+      <c r="A1" t="str">
+        <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
+        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3035,41 +2958,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43682</v>
-      </c>
-      <c r="D5">
-        <v>456.45</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D6">
-        <v>478.32</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C7" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D7">
-        <v>654</v>
+        <v>43590</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3080,10 +2990,7 @@
         <v>177</v>
       </c>
       <c r="C8" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D8">
-        <v>457.5</v>
+        <v>43653</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3091,14 +2998,9 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D9">
-        <v>654</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
@@ -3116,13 +3018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3148,24 +3048,6 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <root xmlns="DBModifDef">
-  <DBActionTest>
-    <env>3</env>
-    <database>ORE</database>
-    <execOnSave>False</execOnSave>
-    <askBeforeExecute>True</askBeforeExecute>
-  </DBActionTest>
-  <DBMapperemployee>
-    <env>3</env>
-    <database>pubs</database>
-    <tableName>employee</tableName>
-    <primKeysStr>emp_id</primKeysStr>
-    <insertIfMissing>True</insertIfMissing>
-    <executeAdditionalProc/>
-    <ignoreColumns/>
-    <execOnSave>False</execOnSave>
-    <CUDFlags>False</CUDFlags>
-    <askBeforeExecute>True</askBeforeExecute>
-  </DBMapperemployee>
   <DBMapperDataRange>
     <env>3</env>
     <database>ORE</database>
@@ -3178,12 +3060,6 @@
     <CUDFlags>False</CUDFlags>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapperDataRange>
-  <DBSeqnceTest>
-    <execOnSave>True</execOnSave>
-    <askBeforeExecute>True</askBeforeExecute>
-    <seqStep>DBAction:DBActionTest</seqStep>
-    <seqStep>DBMapper:DBMapperDataRange</seqStep>
-  </DBSeqnceTest>
   <DBSeqncetestRefresh>
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
@@ -3191,22 +3067,46 @@
     <seqStep>DBRefrsh:DBFsource436717175553588:DBListFetch(in Example2!$A$1)</seqStep>
   </DBSeqncetestRefresh>
   <DBMapper>
-    <env/>
+    <env>3</env>
     <database>ORE</database>
     <tableName>TestTable</tableName>
     <primKeysStr>TestID</primKeysStr>
     <insertIfMissing>True</insertIfMissing>
     <executeAdditionalProc/>
     <ignoreColumns>ignoredColumn</ignoreColumns>
-    <execOnSave>False</execOnSave>
     <CUDFlags>False</CUDFlags>
+    <execOnSave>True</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapper>
+  <DBMapperemployee>
+    <env>3</env>
+    <database>pubs</database>
+    <tableName>employee</tableName>
+    <primKeysStr>emp_id</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns/>
+    <CUDFlags>False</CUDFlags>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapperemployee>
+  <DBActionTest>
+    <env>3</env>
+    <database>ORE</database>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBActionTest>
+  <DBSeqnceTest>
+    <execOnSave>True</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+    <seqStep>DBMapper:DBMapperDataRange</seqStep>
+    <seqStep>DBAction:DBActionTest</seqStep>
+  </DBSeqnceTest>
 </root>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60067F7C-9141-4335-856F-A5078F7B86EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0493CEE7-CD9F-4146-8422-B8D7056C7333}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="DBModifDef"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
added DBBeginTrans and DBCommitTrans
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -18,7 +18,7 @@
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
     <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
     <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$E$9</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
@@ -2547,10 +2547,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2751,6 +2751,24 @@
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2894,7 +2912,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3048,41 +3066,47 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <root xmlns="DBModifDef">
-  <DBMapperDataRange>
-    <env>3</env>
-    <database>ORE</database>
-    <tableName>TestTable</tableName>
-    <primKeysStr>TestID</primKeysStr>
-    <insertIfMissing>True</insertIfMissing>
-    <executeAdditionalProc/>
-    <ignoreColumns/>
-    <execOnSave>False</execOnSave>
-    <CUDFlags>False</CUDFlags>
-    <askBeforeExecute>True</askBeforeExecute>
-  </DBMapperDataRange>
   <DBSeqncetestRefresh>
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
     <seqStep>DBMapper:DBMapperDataRange</seqStep>
     <seqStep>DBRefrsh:DBFsource436717175553588:DBListFetch(in Example2!$A$1)</seqStep>
   </DBSeqncetestRefresh>
+  <DBActionTest>
+    <env>3</env>
+    <database>ORE</database>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBActionTest>
+  <DBMapperDataRange>
+    <env>3</env>
+    <database>ORE</database>
+    <tableName>TestTable</tableName>
+    <primKeysStr>1</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns/>
+    <CUDFlags>False</CUDFlags>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapperDataRange>
   <DBMapper>
     <env>3</env>
     <database>ORE</database>
     <tableName>TestTable</tableName>
-    <primKeysStr>TestID</primKeysStr>
+    <primKeysStr>1</primKeysStr>
     <insertIfMissing>True</insertIfMissing>
     <executeAdditionalProc/>
     <ignoreColumns>ignoredColumn</ignoreColumns>
     <CUDFlags>False</CUDFlags>
-    <execOnSave>True</execOnSave>
+    <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapper>
   <DBMapperemployee>
     <env>3</env>
     <database>pubs</database>
     <tableName>employee</tableName>
-    <primKeysStr>emp_id</primKeysStr>
+    <primKeysStr>1</primKeysStr>
     <insertIfMissing>True</insertIfMissing>
     <executeAdditionalProc/>
     <ignoreColumns/>
@@ -3090,23 +3114,19 @@
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapperemployee>
-  <DBActionTest>
-    <env>3</env>
-    <database>ORE</database>
-    <execOnSave>False</execOnSave>
-    <askBeforeExecute>True</askBeforeExecute>
-  </DBActionTest>
   <DBSeqnceTest>
     <execOnSave>True</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
+    <seqStep>DBBeginTrans:Begin DB Transaction:(only works in same environment)</seqStep>
     <seqStep>DBMapper:DBMapperDataRange</seqStep>
     <seqStep>DBAction:DBActionTest</seqStep>
+    <seqStep>DBCommitTrans:Commit DB Transaction:(only works in same environment)</seqStep>
   </DBSeqnceTest>
 </root>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0493CEE7-CD9F-4146-8422-B8D7056C7333}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A8A02C-363C-45D1-B3A7-884D96369A58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="DBModifDef"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
started transactions fixed dbseqence repairing
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D088F18E-42E9-4F63-B9AC-DEC5FE9F0C44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -16,17 +22,17 @@
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$9</definedName>
-    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$9</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$10</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$13</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$10</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$13</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,15 +50,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
   <si>
     <t>0877</t>
   </si>
@@ -576,18 +582,6 @@
     <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>etertert</t>
-  </si>
-  <si>
-    <t>jkhjkhjk</t>
-  </si>
-  <si>
-    <t>ertert</t>
-  </si>
-  <si>
     <t>ignoredColumn</t>
   </si>
   <si>
@@ -606,13 +600,31 @@
     <t>ttt</t>
   </si>
   <si>
-    <t>AAAA</t>
+    <t>TestId</t>
+  </si>
+  <si>
+    <t>dsfsdfsdfsd</t>
+  </si>
+  <si>
+    <t>rewrwer</t>
+  </si>
+  <si>
+    <t>zrtzrtz</t>
+  </si>
+  <si>
+    <t>rtzrtzrtzrtz</t>
+  </si>
+  <si>
+    <t>rtert</t>
+  </si>
+  <si>
+    <t>jhg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -722,11 +734,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -734,6 +749,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -763,11 +792,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -775,6 +807,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -804,11 +850,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -816,6 +865,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -845,11 +908,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -857,6 +923,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -886,11 +966,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -898,6 +981,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -909,7 +1006,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -922,13 +1019,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D13" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1223,14 +1320,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2509,13 +2606,13 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -2545,17 +2642,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2574,12 +2671,12 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, (last result:)Retrieved 7 records from: select * from ORE..Testtable</v>
+        <v>Env:MSSQL, (last result:)Retrieved 8 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>167</v>
@@ -2591,7 +2688,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -2608,7 +2705,7 @@
         <v>123.9</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2636,7 +2733,7 @@
         <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2655,12 +2752,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+        <v>181</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43682</v>
+      </c>
+      <c r="D5" s="6">
+        <v>456.45</v>
+      </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -2668,12 +2769,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43685</v>
+      </c>
+      <c r="D6" s="6">
+        <v>478.32</v>
+      </c>
+      <c r="E6" t="s">
         <v>175</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
-      <c r="E6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -2681,24 +2786,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C7" s="2">
-        <v>43590</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>43717</v>
+      </c>
+      <c r="D7" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C8" s="2">
-        <v>43653</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>43685</v>
+      </c>
+      <c r="D8" s="6">
+        <v>457.5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -2707,14 +2816,26 @@
       <c r="B9" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="2">
+        <v>43717</v>
+      </c>
+      <c r="D9" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44051</v>
+      </c>
+      <c r="D10" s="6">
+        <v>9879</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -2779,52 +2900,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
+        <control shapeId="1025" r:id="rId4" name="DBMapper">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
+        <control shapeId="1026" r:id="rId6" name="DBActionTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
+        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2854,52 +2975,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId10" name="DBActionTest">
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId12" name="DBMapper">
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2907,17 +3028,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2926,12 +3047,12 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>167</v>
@@ -2976,28 +3097,41 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43682</v>
+      </c>
+      <c r="D5">
+        <v>456.45</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>182</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D6">
+        <v>478.32</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C7" s="3">
-        <v>43590</v>
+        <v>43717</v>
+      </c>
+      <c r="D7">
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3005,10 +3139,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C8" s="3">
-        <v>43653</v>
+        <v>43685</v>
+      </c>
+      <c r="D8">
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3018,11 +3155,48 @@
       <c r="B9" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>43717</v>
+      </c>
+      <c r="D9">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44051</v>
+      </c>
+      <c r="D10">
+        <v>9879</v>
+      </c>
       <c r="G10" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3036,7 +3210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3117,10 +3291,10 @@
   <DBSeqnceTest>
     <execOnSave>True</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
-    <seqStep>DBBeginTrans:Begin DB Transaction:(only works in same environment)</seqStep>
+    <seqStep>DBBegin:Begins DB Transaction</seqStep>
     <seqStep>DBMapper:DBMapperDataRange</seqStep>
     <seqStep>DBAction:DBActionTest</seqStep>
-    <seqStep>DBCommitTrans:Commit DB Transaction:(only works in same environment)</seqStep>
+    <seqStep>DBCommitRollback:Commits or Rolls back DB Transaction</seqStep>
   </DBSeqnceTest>
 </root>
 </file>

</xml_diff>

<commit_message>
fixed Transaction handling revert hidden DBfunction extent in DBListFetch changed dirty setting in refreshData to changing targetcells. fixed problem with invocation of DBModifiers while in edit mode
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D088F18E-42E9-4F63-B9AC-DEC5FE9F0C44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -22,17 +16,17 @@
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$10</definedName>
-    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$13</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$10</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2:$D$13</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$8</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$8</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$8</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$8</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$13</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,15 +44,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="186">
   <si>
     <t>0877</t>
   </si>
@@ -576,9 +570,6 @@
     <t>testtesttest</t>
   </si>
   <si>
-    <t>werwer</t>
-  </si>
-  <si>
     <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
   </si>
   <si>
@@ -600,32 +591,32 @@
     <t>ttt</t>
   </si>
   <si>
-    <t>TestId</t>
-  </si>
-  <si>
-    <t>dsfsdfsdfsd</t>
-  </si>
-  <si>
-    <t>rewrwer</t>
-  </si>
-  <si>
-    <t>zrtzrtz</t>
-  </si>
-  <si>
-    <t>rtzrtzrtzrtz</t>
-  </si>
-  <si>
-    <t>rtert</t>
-  </si>
-  <si>
-    <t>jhg</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>jkhjkhjk</t>
+  </si>
+  <si>
+    <t>ertert</t>
+  </si>
+  <si>
+    <t>AAAA</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>ertertrtt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -633,6 +624,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -658,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -669,13 +666,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,14 +823,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -749,20 +835,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -792,14 +864,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -807,20 +876,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -850,14 +905,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -865,20 +917,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -908,14 +946,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -923,20 +958,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -966,14 +987,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -981,20 +999,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1006,7 +1010,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -1019,13 +1023,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D13" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A2:D8"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4"/>
+    <tableColumn id="1" uniqueName="1" name="Spalte1" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1320,14 +1324,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
@@ -2606,13 +2610,13 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" t="s">
         <v>178</v>
       </c>
-      <c r="B48" t="s">
-        <v>179</v>
-      </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -2642,17 +2646,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -2671,12 +2675,12 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:MSSQL, (last result:)Retrieved 8 records from: select * from ORE..Testtable</v>
+        <v>Env:Development, (last result:)Retrieved 6 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>167</v>
@@ -2688,7 +2692,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -2705,7 +2709,7 @@
         <v>123.9</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2733,7 +2737,7 @@
         <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2749,93 +2753,67 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43682</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="6">
-        <v>456.45</v>
+        <v>345345</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D6" s="6">
-        <v>478.32</v>
-      </c>
+        <v>43590</v>
+      </c>
+      <c r="D6" s="6"/>
       <c r="E6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C7" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D7" s="6">
-        <v>654</v>
-      </c>
+        <v>43653</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="2">
-        <v>43685</v>
-      </c>
-      <c r="D8" s="6">
-        <v>457.5</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="2">
-        <v>43717</v>
-      </c>
-      <c r="D9" s="6">
-        <v>654</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="2">
-        <v>44051</v>
-      </c>
-      <c r="D10" s="6">
-        <v>9879</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -3028,175 +3006,127 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+        <v>Env:Development, (last result:)</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="10">
+        <v>32874</v>
+      </c>
+      <c r="D3" s="9">
+        <v>123.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="10">
+        <v>43586</v>
+      </c>
+      <c r="D4" s="9">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9">
+        <v>345345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="3">
-        <v>32874</v>
-      </c>
-      <c r="D3">
-        <v>123.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="3">
-        <v>43586</v>
-      </c>
-      <c r="D4">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" s="10">
+        <v>43590</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="3">
-        <v>43682</v>
-      </c>
-      <c r="D5">
-        <v>456.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" s="10">
+        <v>43653</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D6">
-        <v>478.32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
         <v>172</v>
-      </c>
-      <c r="C7" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D7">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="3">
-        <v>43685</v>
-      </c>
-      <c r="D8">
-        <v>457.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43717</v>
-      </c>
-      <c r="D9">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="3">
-        <v>44051</v>
-      </c>
-      <c r="D10">
-        <v>9879</v>
-      </c>
-      <c r="G10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3210,7 +3140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3252,18 +3182,6 @@
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBActionTest>
-  <DBMapperDataRange>
-    <env>3</env>
-    <database>ORE</database>
-    <tableName>TestTable</tableName>
-    <primKeysStr>1</primKeysStr>
-    <insertIfMissing>True</insertIfMissing>
-    <executeAdditionalProc/>
-    <ignoreColumns/>
-    <CUDFlags>False</CUDFlags>
-    <execOnSave>False</execOnSave>
-    <askBeforeExecute>True</askBeforeExecute>
-  </DBMapperDataRange>
   <DBMapper>
     <env>3</env>
     <database>ORE</database>
@@ -3288,12 +3206,25 @@
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapperemployee>
+  <DBMapperDataRange>
+    <env>3</env>
+    <database>ORE</database>
+    <tableName>TestTable</tableName>
+    <primKeysStr>1</primKeysStr>
+    <insertIfMissing>True</insertIfMissing>
+    <executeAdditionalProc/>
+    <ignoreColumns/>
+    <CUDFlags>True</CUDFlags>
+    <execOnSave>False</execOnSave>
+    <askBeforeExecute>True</askBeforeExecute>
+  </DBMapperDataRange>
   <DBSeqnceTest>
     <execOnSave>True</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
     <seqStep>DBBegin:Begins DB Transaction</seqStep>
     <seqStep>DBMapper:DBMapperDataRange</seqStep>
     <seqStep>DBAction:DBActionTest</seqStep>
+    <seqStep>DBRefrsh:DBFsource43741663536713:DBSetQuery(in Example3!$A$1)</seqStep>
     <seqStep>DBCommitRollback:Commits or Rolls back DB Transaction</seqStep>
   </DBSeqnceTest>
 </root>

</xml_diff>

<commit_message>
fixed DBRefresh (rewritten as "manual" invocation of DBFunctions)
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,12 @@
     <definedName name="DBActionTest">ExampleDBAction!$A$1</definedName>
     <definedName name="DBFsource436717175553588" hidden="1">Example2!$A$1</definedName>
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
+    <definedName name="DBFsource438884830419676" hidden="1">Example2!#REF!</definedName>
+    <definedName name="DBFsource438885783299074" hidden="1">Example2!#REF!</definedName>
     <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$8</definedName>
     <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$8</definedName>
+    <definedName name="DBFtarget438884830419676" hidden="1">Example2!#REF!</definedName>
+    <definedName name="DBFtarget438885783299074" hidden="1">Example2!#REF!</definedName>
     <definedName name="DBMapper">Example2!$A$2:$D$8</definedName>
     <definedName name="DBMapperDataRange">Example3!$A$2:$D$8</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="184">
   <si>
     <t>0877</t>
   </si>
@@ -601,12 +605,6 @@
   </si>
   <si>
     <t>AAAA</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>Spalte1</t>
   </si>
   <si>
     <t>ertertrtt</t>
@@ -616,7 +614,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -624,12 +622,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -655,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -666,10 +658,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -678,7 +668,7 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i/>
+        <i val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1023,10 +1013,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A2:D8"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Spalte1" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4" dataDxfId="2"/>
@@ -1324,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2648,10 +2638,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2663,22 +2653,16 @@
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
         <v>Env:Development, (last result:)Retrieved 6 records from: select * from ORE..Testtable</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>179</v>
       </c>
@@ -2695,7 +2679,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2716,14 +2700,8 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2744,19 +2722,13 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6">
@@ -2766,7 +2738,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2781,7 +2753,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2793,7 +2765,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2801,51 +2773,53 @@
         <v>182</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D8" s="6">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="2"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="2"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
@@ -2878,52 +2852,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="DBMapper">
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
+        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="DBActionTest">
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
+        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2953,52 +2927,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
+        <control shapeId="1026" r:id="rId10" name="DBActionTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
+        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
+        <control shapeId="1025" r:id="rId12" name="DBMapper">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3010,27 +2984,27 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, (last result:)</v>
+        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>167</v>
@@ -3041,73 +3015,70 @@
       <c r="D2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="9">
+        <v>32874</v>
+      </c>
+      <c r="D3" s="8">
+        <v>123.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="9">
+        <v>43586</v>
+      </c>
+      <c r="D4" s="8">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="10">
-        <v>32874</v>
-      </c>
-      <c r="D3" s="9">
-        <v>123.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="10">
-        <v>43586</v>
-      </c>
-      <c r="D4" s="9">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9">
+      <c r="C5" s="9"/>
+      <c r="D5" s="8">
         <v>345345</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>43590</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>43653</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
@@ -3116,12 +3087,9 @@
       <c r="B8" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" t="s">
-        <v>183</v>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8">
+        <v>897</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed callid missing bug fixed targetRange not reference problem fixed inserting/updating null values problem
</commit_message>
<xml_diff>
--- a/test/DBMapperTests.xlsx
+++ b/test/DBMapperTests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr codeName="DieseArbeitsmappe"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1B976-E5CE-40FD-BAE6-A5D6EAEA2FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
@@ -18,19 +24,33 @@
     <definedName name="DBFsource43741663536713" hidden="1">Example3!$A$1</definedName>
     <definedName name="DBFsource438884830419676" hidden="1">Example2!#REF!</definedName>
     <definedName name="DBFsource438885783299074" hidden="1">Example2!#REF!</definedName>
-    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$8</definedName>
-    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$8</definedName>
+    <definedName name="DBFsource438898127587384" hidden="1">Example3!$J$1</definedName>
+    <definedName name="DBFtarget436717175553588" hidden="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="DBFtarget43741663536713" hidden="1">Example3!$A$2:$D$9</definedName>
     <definedName name="DBFtarget438884830419676" hidden="1">Example2!#REF!</definedName>
     <definedName name="DBFtarget438885783299074" hidden="1">Example2!#REF!</definedName>
-    <definedName name="DBMapper">Example2!$A$2:$D$8</definedName>
-    <definedName name="DBMapperDataRange">Example3!$A$2:$D$8</definedName>
+    <definedName name="DBFtarget438898127587384" hidden="1">Example3!$J$2:$K$9</definedName>
+    <definedName name="DBMapper">Example2!$A$2:$D$11</definedName>
+    <definedName name="DBMapperDataRange">Example3!$A$2:$D$9</definedName>
     <definedName name="DBMapperemployee">Example1!$A$1:$H$48</definedName>
     <definedName name="DBSeqnce">ExampleDBAction!$A$3</definedName>
     <definedName name="employee">Example1!$A$1:$H$47</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1">Example2!$A$2:$D$12</definedName>
-    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$8</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="2" hidden="1">Example3!$J$2:$K$9</definedName>
+    <definedName name="ExterneDaten_10" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_11" localSheetId="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="ExterneDaten_12" localSheetId="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="ExterneDaten_2" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_3" localSheetId="1">Example2!$A$2:$D$12</definedName>
+    <definedName name="ExterneDaten_4" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_5" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_6" localSheetId="1">Example2!$A$2:$D$11</definedName>
+    <definedName name="ExterneDaten_7" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_8" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="ExterneDaten_9" localSheetId="1">Example2!$A$2:$D$9</definedName>
+    <definedName name="OEBFADBTVI00_ORE_TestTable" localSheetId="2" hidden="1">Example3!$A$2:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,15 +68,18 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="TestTable" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="Select * FROM ORE..TestTable"/>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="TestTable" type="5" refreshedVersion="6" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select * FROM ORE..TestTable"/>
+  </connection>
+  <connection id="2" xr16:uid="{E107CA91-87EA-4FB1-96DC-0F806182D31F}" keepAlive="1" name="Verbindung" type="5" refreshedVersion="6" background="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL SERVER;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="Select TestStr,TestId FROM ORE..TestTable"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="186">
   <si>
     <t>0877</t>
   </si>
@@ -571,9 +594,6 @@
     <t>testtest</t>
   </si>
   <si>
-    <t>testtesttest</t>
-  </si>
-  <si>
     <t>mapper.saveRangeToDBSingle(Range("testLegacyName"), "TestTable", "TestID", "MSSQLORE", True)</t>
   </si>
   <si>
@@ -595,25 +615,34 @@
     <t>ttt</t>
   </si>
   <si>
-    <t>TestID</t>
-  </si>
-  <si>
-    <t>jkhjkhjk</t>
-  </si>
-  <si>
-    <t>ertert</t>
-  </si>
-  <si>
-    <t>AAAA</t>
-  </si>
-  <si>
-    <t>ertertrtt</t>
+    <t>TestId</t>
+  </si>
+  <si>
+    <t>dsfsdfsdfsd</t>
+  </si>
+  <si>
+    <t>rewrwer</t>
+  </si>
+  <si>
+    <t>werwer</t>
+  </si>
+  <si>
+    <t>zrtzrtz</t>
+  </si>
+  <si>
+    <t>rtzrtzrtzrtz</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>ghjgjhg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -677,6 +706,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -692,6 +722,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -707,6 +738,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -722,6 +754,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
@@ -738,6 +771,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -753,6 +787,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -813,11 +848,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -825,6 +863,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -854,11 +906,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -866,6 +921,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -895,11 +964,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -907,6 +979,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -936,11 +1022,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -948,6 +1037,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -977,11 +1080,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -989,6 +1095,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1000,7 +1120,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="OEBFADBTVI00 ORE TestTable" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="OEBFADBTVI00 ORE TestTable" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="TestID" tableColumnId="1"/>
@@ -1012,14 +1132,36 @@
 </queryTable>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="2" xr16:uid="{3949D603-2368-4F66-9B82-E284A6496A50}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="4">
+    <queryTableFields count="2">
+      <queryTableField id="2" name="TestStr" tableColumnId="3"/>
+      <queryTableField id="3" name="TestId" tableColumnId="4"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestTable" displayName="TestTable" ref="A2:D8" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TestTable" displayName="TestTable" ref="A2:D9" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="TestID" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" uniqueName="2" name="TestStr" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" uniqueName="4" name="TestNum" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="TestId" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="TestStr" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="TestDate" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="TestNum" queryTableFieldId="4" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3265ECDB-2EA0-4DB0-80A0-F3B0CC429330}" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="J2:K9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="J2:K9" xr:uid="{A9CB6152-2971-427B-B6E2-4A2C144C5B77}"/>
+  <tableColumns count="2">
+    <tableColumn id="3" xr3:uid="{F975AAF0-D4F2-4E8F-ABEE-9D885F9D414F}" uniqueName="3" name="TestStr" queryTableFieldId="2"/>
+    <tableColumn id="4" xr3:uid="{2B0A4078-8369-442E-917A-94507FF1C136}" uniqueName="4" name="TestId" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1314,20 +1456,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1600,6 +1742,9 @@
       <c r="H10" s="2">
         <v>33537</v>
       </c>
+      <c r="L10" t="s">
+        <v>171</v>
+      </c>
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -2600,13 +2745,13 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s">
         <v>177</v>
       </c>
-      <c r="B48" t="s">
-        <v>178</v>
-      </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -2636,18 +2781,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -2659,12 +2804,12 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBListFetch("select * from ORE..Testtable",3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, (last result:)Retrieved 6 records from: select * from ORE..Testtable</v>
+        <v>Env:MSSQL, (last result:)Retrieved 9 records from: select * from ORE..Testtable</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>167</v>
@@ -2676,7 +2821,7 @@
         <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2693,7 +2838,7 @@
         <v>123.9</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2706,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C4" s="2">
         <v>43586</v>
@@ -2715,7 +2860,7 @@
         <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2725,72 +2870,88 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43682</v>
+      </c>
       <c r="D5" s="6">
-        <v>345345</v>
+        <v>456.45</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>180</v>
       </c>
       <c r="C6" s="2">
-        <v>43590</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>43685</v>
+      </c>
+      <c r="D6" s="6">
+        <v>478.32</v>
+      </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="2">
-        <v>43653</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6">
-        <v>897</v>
+        <v>457.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>183</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6">
+        <v>654</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>185</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
@@ -2852,52 +3013,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest">
+        <control shapeId="1025" r:id="rId4" name="DBMapper">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="DBSeqnceTest"/>
+        <control shapeId="1025" r:id="rId4" name="DBMapper"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee">
+        <control shapeId="1026" r:id="rId6" name="DBActionTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId6" name="DBMapperemployee"/>
+        <control shapeId="1026" r:id="rId6" name="DBActionTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2927,52 +3088,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId10" name="DBActionTest">
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId10" name="DBActionTest"/>
+        <control shapeId="1028" r:id="rId10" name="DBMapperemployee"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId12" name="DBMapper">
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId12" name="DBMapper"/>
+        <control shapeId="1029" r:id="rId12" name="DBSeqnceTest"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2980,31 +3141,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xll.DBSetQuery("Select * FROM ORE..TestTable",3,A2)</f>
-        <v>Env:Development, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select * FROM ORE..TestTable</v>
+      </c>
+      <c r="J1" t="str">
+        <f>_xll.DBSetQuery("Select TestStr,TestId FROM ORE..TestTable",3,J2)</f>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= True): Select TestStr,TestId FROM ORE..TestTable</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>167</v>
@@ -3015,8 +3183,14 @@
       <c r="D2" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -3029,13 +3203,19 @@
       <c r="D3" s="8">
         <v>123.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C4" s="9">
         <v>43586</v>
@@ -3043,72 +3223,120 @@
       <c r="D4" s="8">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="9">
+        <v>43682</v>
+      </c>
+      <c r="D5" s="8">
+        <v>456.45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
         <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8">
-        <v>345345</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>180</v>
       </c>
       <c r="C6" s="9">
-        <v>43590</v>
-      </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43685</v>
+      </c>
+      <c r="D6" s="8">
+        <v>478.32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="9">
-        <v>43653</v>
-      </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="9"/>
+      <c r="D7" s="8">
+        <v>654</v>
+      </c>
+      <c r="J7" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>182</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="8">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>172</v>
+        <v>457.5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8">
+        <v>654</v>
+      </c>
+      <c r="J9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3138,12 +3366,6 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <root xmlns="DBModifDef">
-  <DBSeqncetestRefresh>
-    <execOnSave>False</execOnSave>
-    <askBeforeExecute>True</askBeforeExecute>
-    <seqStep>DBMapper:DBMapperDataRange</seqStep>
-    <seqStep>DBRefrsh:DBFsource436717175553588:DBListFetch(in Example2!$A$1)</seqStep>
-  </DBSeqncetestRefresh>
   <DBActionTest>
     <env>3</env>
     <database>ORE</database>
@@ -3183,6 +3405,7 @@
     <executeAdditionalProc/>
     <ignoreColumns/>
     <CUDFlags>True</CUDFlags>
+    <IgnoreDataErrors>False</IgnoreDataErrors>
     <execOnSave>False</execOnSave>
     <askBeforeExecute>True</askBeforeExecute>
   </DBMapperDataRange>
@@ -3192,14 +3415,15 @@
     <seqStep>DBBegin:Begins DB Transaction</seqStep>
     <seqStep>DBMapper:DBMapperDataRange</seqStep>
     <seqStep>DBAction:DBActionTest</seqStep>
+    <seqStep>DBCommitRollback:Commits or Rolls back DB Transaction</seqStep>
+    <seqStep>DBRefrsh:DBFsource438898127587384:DBSetQuery(in Example3!$J$1)</seqStep>
     <seqStep>DBRefrsh:DBFsource43741663536713:DBSetQuery(in Example3!$A$1)</seqStep>
-    <seqStep>DBCommitRollback:Commits or Rolls back DB Transaction</seqStep>
   </DBSeqnceTest>
 </root>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A8A02C-363C-45D1-B3A7-884D96369A58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CF05E2C-BFD9-46F7-AB09-F4D0E09A57D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="DBModifDef"/>
   </ds:schemaRefs>

</xml_diff>